<commit_message>
Reservation Controller + Validations
</commit_message>
<xml_diff>
--- a/ParkingApp.Main/src/ParkingApp.Main.Common/Files/PublicParkingSpots.xlsx
+++ b/ParkingApp.Main/src/ParkingApp.Main.Common/Files/PublicParkingSpots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\LICENTA\ParkingApp\ParkingApp.Main\src\ParkingApp.Main.Common\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2B3B058-C77D-4625-BA86-817D6E368E7A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22913AF-E207-45B4-9EF8-D5101D46FBAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>PricePerHour</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Sector 5</t>
+  </si>
+  <si>
+    <t>AvailableSpots</t>
   </si>
 </sst>
 </file>
@@ -423,21 +426,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="18.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.88671875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="5" width="8.88671875" style="2"/>
+    <col min="6" max="6" width="18.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -445,22 +448,25 @@
         <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -468,23 +474,26 @@
         <v>96</v>
       </c>
       <c r="C2" s="2">
+        <v>96</v>
+      </c>
+      <c r="D2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -492,19 +501,22 @@
         <v>29</v>
       </c>
       <c r="C3" s="2">
-        <v>3.99</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -512,22 +524,25 @@
         <v>8</v>
       </c>
       <c r="C4" s="2">
-        <v>5.99</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -535,22 +550,25 @@
         <v>59</v>
       </c>
       <c r="C5" s="2">
-        <v>4.99</v>
-      </c>
-      <c r="D5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -558,15 +576,18 @@
         <v>56</v>
       </c>
       <c r="C6" s="2">
-        <v>9.99</v>
-      </c>
-      <c r="D6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first functionality of app
</commit_message>
<xml_diff>
--- a/ParkingApp.Main/src/ParkingApp.Main.Common/Files/PublicParkingSpots.xlsx
+++ b/ParkingApp.Main/src/ParkingApp.Main.Common/Files/PublicParkingSpots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\facultate\LICENTA\ParkingApp\ParkingApp.Main\src\ParkingApp.Main.Common\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22913AF-E207-45B4-9EF8-D5101D46FBAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08AF855-7652-407D-86F4-D8580EA56E82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>PricePerHour</t>
   </si>
@@ -85,13 +85,34 @@
   </si>
   <si>
     <t>AvailableSpots</t>
+  </si>
+  <si>
+    <t>Alexandru Constantinescu</t>
+  </si>
+  <si>
+    <t>INTRE BD. MARASESTI SI BD. ION MIHALACHE</t>
+  </si>
+  <si>
+    <t>STR. PICTOR VERONA, INTRE BD. MAGHERU SI STR. PITAR MOS</t>
+  </si>
+  <si>
+    <t>Calea Rahovei</t>
+  </si>
+  <si>
+    <t>INTRE BD. LIBERTATII SI STR. SABINELOR</t>
+  </si>
+  <si>
+    <t>Pictor Verona</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,17 +129,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF0A0A0A"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0A0A0A"/>
+      <name val="Poppins"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0A0A0A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0A0A0A"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -138,17 +189,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Virgulă" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -426,173 +496,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="5" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="3" width="8.88671875" style="3"/>
+    <col min="4" max="4" width="8.88671875" style="5"/>
+    <col min="5" max="5" width="8.88671875" style="2"/>
     <col min="6" max="6" width="18.88671875" style="2" customWidth="1"/>
-    <col min="7" max="7" width="21.88671875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="21.88671875" style="6" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+    <row r="2" spans="1:9">
+      <c r="A2" s="11">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="12">
         <v>96</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="12">
         <v>96</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="3" spans="1:9">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="12">
         <v>29</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="12">
         <v>29</v>
       </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="13">
+        <v>0</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="G3" s="15"/>
+      <c r="H3" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+    <row r="4" spans="1:9">
+      <c r="A4" s="11">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="12">
         <v>8</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="12">
         <v>8</v>
       </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="D4" s="13">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="H4" s="11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+    <row r="5" spans="1:9">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="12">
         <v>59</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="12">
         <v>59</v>
       </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="13">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+    <row r="6" spans="1:9">
+      <c r="A6" s="11">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="12">
         <v>56</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="12">
         <v>56</v>
       </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="D6" s="13">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="G6" s="15"/>
+      <c r="H6" s="11" t="s">
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="11">
+        <v>6</v>
+      </c>
+      <c r="B7" s="17">
+        <v>153</v>
+      </c>
+      <c r="C7" s="17">
+        <v>153</v>
+      </c>
+      <c r="D7" s="18">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="11">
+        <v>7</v>
+      </c>
+      <c r="B8" s="12">
+        <v>41</v>
+      </c>
+      <c r="C8" s="12">
+        <v>41</v>
+      </c>
+      <c r="D8" s="18">
+        <v>0</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="11">
+        <v>8</v>
+      </c>
+      <c r="B9" s="12">
+        <v>107</v>
+      </c>
+      <c r="C9" s="12">
+        <v>107</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="11"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="11"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="11"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="11"/>
+    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>